<commit_message>
fix set_number_format for columns
</commit_message>
<xml_diff>
--- a/test/numeric_format_test.xlsx
+++ b/test/numeric_format_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krakotay\Documents\rust\xlsx-quick-append-rs\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1F6C30-77B3-45BC-B7FB-251B80BF9910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E2013-F17C-40D2-98F4-A6485BEB1670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,18 +38,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +60,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -351,7 +345,7 @@
   <dimension ref="A3:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>